<commit_message>
Get daily reddit data: Tue Dec 12 08:08:27 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_12_17.xlsx
+++ b/data/2023_12_17.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C457"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,2658 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>18gg75p</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>different account, same nails 💅</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gg75p</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>18g4sc5</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Small nail update</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18g4sc5</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>18gewfl</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>After 13 hours...Christmas Nails Complete</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gewfl</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>18gekfi</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Classic french on natural nails</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gekfi</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>18ge93t</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>HELP! Can press one be taken off quickly?</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ge93t</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>18gdvu2</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>XMAS GIFT HELP NEEDED</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18gdvu2/xmas_gift_help_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>18gde9d</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>I love how these turned out!</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gde9d</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>18gd5p9</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Acrylic full set</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2x4n1gjhgs5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>18gd0nx</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Recently got gifted this nail polish caddy and am in LOVE</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i3zxcms7fs5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>18gcrko</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Blush glitter almonds</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gcrko</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>18gclck</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Bday nails from last month 🎨</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gclck</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>18gcgk0</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Christmas nails🎄</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3gaf6vlr9s5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>18gc8p5</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>I have hands of a worker. But I still enjoy having long nails. New place did a good job on my Christmas nails?</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/54hh52gn7s5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>18gc7go</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Sugar Plum Christmas Nails :)</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a0olzqsb7s5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>18gbzej</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>My natural nails need help</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j6bp3a485s5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>18gbp3r</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>2nd Christmas set I did myself!</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gbp3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>18gbkct</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>My Holiday Nails! 🎄</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gbkct</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>18gbjgv</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>OPI repair mode / how many times a day is too much?</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18gbjgv/opi_repair_mode_how_many_times_a_day_is_too_much/</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>18gaxx2</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>I decided to try shorter nails!</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gaxx2</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>18gafdf</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>i love seeing the nail growth progress whenever i remove old nail polish 🥰</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gafdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>18ga9ui</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>‘tis the season!! 🎅🎄</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ga9ui</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>18ga106</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>All glitter for these holidays!!</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7zpgmq6lnr5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>18g9r83</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>A husband on a mission. My ladies have been keeping me busy.</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18g9r83</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>18g9f2z</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Holiday Press On Nails</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eonxz6b5ir5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>18g9bjg</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Gift ideas for a nail tech?</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18g9bjg/gift_ideas_for_a_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>18g96fb</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>is my nail salon ruining my nails?</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18g96fb/is_my_nail_salon_ruining_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>18g8v4g</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Shimmery frost princess 💖</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18g8v4g</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>18g8bkv</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Birthday Nails :3</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rwlzs1uq8r5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>18g7wrb</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>I love a super light pink 🥰💓🌸💖💕</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q4sanmla5r5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>18g7v7p</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Week 1 of Christmas Nails......</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gegf8yfv4r5c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>18g78v5</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Winter Cateye</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18g78v5</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>18g77qw</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Gel Nails once a week</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18g77qw/gel_nails_once_a_week/</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>18g6frf</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Cuticle on sides won’t go away no matter how much I nip, buff, and push )):</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ks2pjh1ptq5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>18g6fku</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Left hand is glitter confetti. Right hand is just glitter, but layered. What do you guys think?</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z3upzlontq5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>18g610h</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Just finished my holiday nails!</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18g610h</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>18g4xv7</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Christmas Tiiiime</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18g4xv7</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>18g4uhy</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>My first attempt at aurora nails</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6a0wusd0iq5c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>18g4iao</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>My take on subtle Christmas nails (they look like Mickeys lol)</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18g4iao</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>18g3h6j</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Hand painted / made winter patterns❄️🎄</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/se97hioy7q5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>18g3dey</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Reminds me of Narnia fsr… [winter nails]</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18g3dey</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>18g3cg1</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Sea</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18g3cg1/sea/</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>18g2rte</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Second set of Christmas nails done ... Added my first set to the gallery too because I don't know which I prefer hehe .... Didn't realise how identical the pics were either haha</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18g2rte</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>18g2h95</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Obsessed with my fresh Christmas set</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ejla49yq0q5c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>18g24ry</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Are these nails not good?</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zxlfvv9ayp5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>18g1tfw</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Feedback greatly appreciated?</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/95fcq2h1wp5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>18g0y9q</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My birthday nails! Cat eye/velvet effect. </t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cxn8j4ispp5c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>18g0to0</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>brown chrome struggle</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18g0to0/brown_chrome_struggle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>18g0s0l</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Gel-X Nightmare before Christmas set</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sufbjihjop5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>18fyt4m</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>happy hannukah!</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18fyt4m</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>18g05g5</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Hi! I'm a Dad with a gift recommendation question</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18g05g5/hi_im_a_dad_with_a_gift_recommendation_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>18fzzbs</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>How do good nail techs with good practices exist and where do you find them?</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18fzzbs/how_do_good_nail_techs_with_good_practices_exist/</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>18fzjwz</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>New nails. Love the design myself</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ff1dygw68p5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>18fyxed</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>What’s the best nail shape?</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18fyxed/whats_the_best_nail_shape/</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>18fyj9s</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>tried to do serious nail art, but I think I overdid it… and I don’t know how to do my right hand now either 😭😭</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18fyj9s</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>18fy015</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Looking for a new nail place! - Charleston, SC</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18fy015/looking_for_a_new_nail_place_charleston_sc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>18fvtxt</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>The purple holo gradient of my dreams 💜✨</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18fvtxt</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>18fv5il</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>I did poly gel nails for the first time how did i do</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/baxq0vx89o5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>18fuz12</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>First time shaping my nails</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9zak1srn7o5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>18fux3p</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Abstract Hanukkah nails 💙</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18fux3p</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>18fuj3w</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>🦊</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18fuj3w</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>18fu4as</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Autumnal nails from a while back</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kryhxvrmzn5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>18ftg7z</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>New Christmas set ✨️ I wish I had a more contrasting glittery gold.</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ftg7z</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>18ftbg0</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>May anyone find a dupe for this nail polish ?</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/46td5firrn5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>18fsjyj</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Press on sizing</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18fsjyj/press_on_sizing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>18fsizo</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Wintery Nails ❄️⛄️</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18fsizo</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>18fr38y</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Acrylic overlay over my natural nails!</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h04ag3442n5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>18fqqzf</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Trying out nail stickers</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18fqqzf</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>18fqlpv</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Emerald green gel manicure on short nails</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6vj9vab1wm5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>18fqhwd</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>What do you think about this type of male design?</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/16vzkdloum5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>18fqhnb</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Acrylic falling off?</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18fqhnb</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>18fpo1m</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Cat eye french tip</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/006xm1wsjm5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>18fl50a</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Press on nail that won’t damage?</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18fl50a/press_on_nail_that_wont_damage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>18fk9aw</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Don’t know how to fix my toes!</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18fk9aw/dont_know_how_to_fix_my_toes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>18gdkjt</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Is this what it’s like being in love with a polish?</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gdkjt</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>18gd982</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Thank you whoever posted the fridge magnet trick for velvet nails, you saved me $17! It works!</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q4mkg9yehs5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>18gd8j1</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>took the ilnp plunge</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gd8j1</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>18gcvak</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Nail stamping advice</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18gcvak/nail_stamping_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>18gcnsk</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Kiss Me, even more!!</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gcnsk</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>18gas9u</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Acquired a lab vortexer, am supreme mixer now</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ozmvz2vfur5c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>18gan52</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>marsala jelly!</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gan52</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>18galwf</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Deep true reds?</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18galwf</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>18gahpc</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Funny coincidence while shopping today</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gahpc</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>18g9hmt</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Need advice for home gel manicures</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18g9hmt/need_advice_for_home_gel_manicures/</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>18g9b3p</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>To the person who suggested ordering swatch colors by hue</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kzmmsut5hr5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>18g989g</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Played around with AI to create Christmas nail art</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18g989g</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>18g8ric</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>So delicate and magical ✨</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18g8ric</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>18g8ppz</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Everything is finally organized 😍</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gqj8gro1cr5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>18g89wc</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Finals are over. Celebration nails</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18g89wc</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>18g7r3r</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>the last of my Cyber Monday purchases is here!</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yp6pcg4z3r5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>18g7mdl</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>cirque mother of pearl alternative?</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18g7mdl</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>18g760j</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Morgan Taylor Scandalous ❤️🌹❤️</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qm0kj0bazq5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>18g6td0</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18g6td0</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>18g6pky</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Replacement brush question</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18g6pky/replacement_brush_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>18g6lnv</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Any recommendations on a tackle box for storing nail charms?</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18g6lnv/any_recommendations_on_a_tackle_box_for_storing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>18g6grz</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Death Valley Nails Snake Oil</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4dqcd89xtq5c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>18g6f67</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Stained Glass mysteries</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18g6f67</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>18g629m</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Bigger bottles of smoothing base?</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18g629m/bigger_bottles_of_smoothing_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>18g584z</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🍋 🤤 </t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3qjjfx3rkq5c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>18g57oc</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Mani inspired by my Christmas tree so it still counts as a holiday look ✨</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xmbnp0pokq5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>18g55p1</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Weekly Check-In for those on a no-buy, low-buy, etc.</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18g55p1/weekly_checkin_for_those_on_a_nobuy_lowbuy_etc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>18g4zsu</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>No-Foil Aurora Nails!</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/elydtgk0jq5c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>18g4pi0</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Nothing exciting, but proud of my cuticles!</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v4e76wf1hq5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>18g4o3s</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>A classic black polish 🖤</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18g4o3s</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>18g4mvt</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Zoya Rosalind</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18g4mvt</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>18g4jwd</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Zoya Charla</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18g4jwd</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>18g45n9</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Poshe Top Coat Brush replacement recommendations</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n58fyjwscq5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>18g3obd</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>This is so satisfying! ILNP Deep Space</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i4okip7f9q5c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>18g2i7p</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Went for a pallet cleanser but think I found wedding polish 🤍✨</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18g2i7p</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>18g1ukc</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>How long does a magnetized manicure effect last for you?</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18g1ukc/how_long_does_a_magnetized_manicure_effect_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>18g193i</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Seche Vite, thoughts?</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18g193i/seche_vite_thoughts/</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>18g16l1</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>There’s no party like a pixie party 🧚 🎉</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18g16l1</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>18g14yn</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Opinions on green polish?</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7rldal25rp5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>18g0bx2</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>PSA Cupcake Paddle brushes have been restocked</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cfuq9w4clp5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>18g0bbe</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>We all know Twisted Terracotta Tanzanite is amazing, but did we know…</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q49rzgh7lp5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>18g0a22</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Love Language</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5m22c5yxkp5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>18fzq2h</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Candy Cane Stripes!</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ivena0fh9p5c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>18fzbtw</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>First time going to a salon in nearly a decade</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18fzbtw</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>18fz4n9</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>A lil disappointed with Sweet Pea</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18fz4n9</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>18fys7m</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Super excited about my first attempt colorful French tips!</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18fys7m</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>18fyru2</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Butterfly Nails</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/if5lr8l92p5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>18fyccp</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>My concert nails (plus a shot in regular lighting)</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18fyccp</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>18fy4c9</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>You guys are the best influence.</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0h6he1m8xo5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>18fxud2</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Would someone recommend "olive friendly" peachy nail polishes?</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18fxud2/would_someone_recommend_olive_friendly_peachy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>18fxmpr</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>🩵💙Lilo &amp; Stitch❤️🌴</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18fxmpr</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>18fxemh</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Desperate for dupe recs!</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18fxemh</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>18fx6l2</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Prugly Love - Alchemy Oddities</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7bk1cu1spo5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>18fx5y8</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Polished for Days holiday haul</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18fx5y8</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>18fwyvy</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>♀️ Crushing on Girl Crush 💟</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18fwyvy</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>18fwqjp</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Palate cleanser featuring more Black Friday polishes</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18fwqjp</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>18fwqj2</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Zoya Naked Manicure</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18fwqj2/zoya_naked_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>18fwo30</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Bill!</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/posu9nkulo5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>18fwie4</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>first ILNP order came in just in time for my birthday this weekend 🥳</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18fwie4</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>18fwbqt</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Sorry for the claw hand pose, but trying to show the thumb of this holiday mani 😅</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18fwbqt</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>18fvqms</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Purple holo gradation of my dreams 💜 ✨</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18fvqms</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>18fv8pl</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Nothing like a bright pink holo!</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j7lgdhey9o5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>18fusi5</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>(PR) Abstract Hanukkah nails 💙</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18fusi5</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>18ftgj5</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Monarch - Icy Meadow ❄️</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ftgj5</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>18ft2uu</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Should you use nail strengthener if your nails are already hard and strong?</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18ft2uu/should_you_use_nail_strengthener_if_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>18fs1m8</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18fs1m8/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>18ggmwr</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>love the glitter (gel polish)✨✨✨✨</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2cydc7egit5c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>18ggm6z</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>My nails last week. Gingerbread and GirlyPop Christmas.</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ggm6z</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>18gcdci</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Christmas set done by me</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gcdci</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>18g8k74</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Growing</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9hc5rxupar5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>18g6jal</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Christmas 2023</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vndkh96guq5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>18g5win</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Holiday Nails</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/chqjb9nopq5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>18g4nru</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>My first Halloween set</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18g4nru</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>18g43h0</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Something a lil holly jolly ❤️</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dqmi8f9jcq5c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>18g2dwy</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>First time trying nail art</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18g2dwy</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>18fye1j</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Dripping ice cream Birthday nails!</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ogp8dsazo5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>18fxqfx</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>I've been doing my nails since June. I think these look pretty good 💖 I'm getting better.</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18fxqfx</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>18fvsj2</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>I thought these look like yummy candies. What do you think?</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18fvsj2</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>18furdr</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas Nails </t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xaz6kqwq5o5c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>18fqqdv</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>So much fun omg</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gd8zkfloxm5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>18fqome</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>My first time trying out nail foils…</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18fqome</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>18fqnl8</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>I love gems🥰</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18fqnl8</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>18fqib2</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>What do you think about male nail design like this?</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7d27i2itum5c1.jpg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Dec 13 08:08:14 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_12_17.xlsx
+++ b/data/2023_12_17.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C457"/>
+  <dimension ref="A1:C614"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8202,6 +8202,2675 @@
         </is>
       </c>
     </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>18hbect</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>I’ve done my Christmas Nails 💅</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n4kjl4nvk06c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>18hb2w1</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cve3nf1yg06c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>18haod6</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>First time getting foil nails 💫</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/av335f47c06c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>18ham05</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Am I doing something wrong?</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wl6is3ceb06c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>18h9smj</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Nail the perfect look with 10 paid nail books – now yours for free!</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rzf1ia87206c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>18h74ey</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Can't get a reapplied press on nail to stay?</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18h74ey/cant_get_a_reapplied_press_on_nail_to_stay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>18h3qsw</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>First time doing my own nails - shaping and polish (regular not gel) + HK stickers</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gnl89il3py5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>18h7uru</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>monster ink and toy story</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18h7uru</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>18h7s67</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>My Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18h7s67</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>18h7r25</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Help I need advice :-/</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18h7r25</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>18h6h89</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Solid gel glue</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18h6h89/solid_gel_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>18h61rr</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Glitzy Christmas gel</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1hzeecil2z5c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>18h5sqi</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>First gel x and I HATE them</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18h5sqi</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>18h5quf</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Too basic or just right?</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18h5quf</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>18h5djn</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Festive but make it warm</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pu8tn9wkyy5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>18h5azk</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>First time gel x and I HATE them</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pnvgmyy4yy5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>18h527l</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Red Cat eye pearl (gel-x)</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l4xq3t5pwy5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>18h51cc</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Newbie advice needed</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18h51cc/newbie_advice_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>18h4l7s</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Bestie is a nail tech</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xbmc0cgyty5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>18h47cl</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Found $2 crackle polish 💔💔💔 they look so silly</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18h47cl</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>18h3zyr</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>growth of more than a month, I need a new set of nails :)</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nbbvjo3kqy5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>18h3uz9</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>What winter nail colors suit darker skin that isn’t a neutral pink</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18h3uz9/what_winter_nail_colors_suit_darker_skin_that/</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>18h3rs7</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Question</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18h3rs7/question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>18h3n9k</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>My take on festive nails 🤍🖤</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18h3n9k</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>18gynrh</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Why do professional nailcutters or healthcare professionals with specialist training in clipping nails exist? Why do even normal able bodied people use their services?</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18gynrh/why_do_professional_nailcutters_or_healthcare/</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>18h0uwf</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Christmas set but make it minimal ✨</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jqqfbw019y5c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>18h0aya</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Scared about first nail salon experience</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18h0aya/scared_about_first_nail_salon_experience/</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>18h04vl</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>🎶I’m dreaming of a white Christmas🎶</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w9as6lh15y5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>18gz6yb</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>First Gelx Xmas set</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6qomf7mzzx5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>18gyyaf</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>New DiY Gel set Nude and Gold 💖</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gyyaf</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>18gypvw</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Are thick nails in style now? Meaning there are a lot of coats applied to the nail.</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18gypvw/are_thick_nails_in_style_now_meaning_there_are_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>18gyop4</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>makeup artist here! this was the first time doing my own gel x nails! i’m so proud of how they turned out</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sqvy3vmcxx5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>18gyb1a</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>simple snowflake set ❄️</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gyb1a</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>18gxuni</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>christmas set ! 💚❤️💚</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gxuni</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>18gxnqq</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>My nail tech is actually insane omg</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gxnqq</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>18gxkjj</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Polish chipped and nail tech filed it off</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18gxkjj/polish_chipped_and_nail_tech_filed_it_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>18gxfmt</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>What do you think of my new set? Yay or nay?</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gxfmt</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>18gx2ls</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Short nails can be pretty too❤️</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/larra7alnx5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>18gwtsq</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>This polish is way way more awesome in person. Riviera Rave by I Scream Nails</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gwtsq</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>18gwr99</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Some blue chromey snowflakes</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t25kivc5lx5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>18gwi0r</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Back again for round two on the nail gem critique!</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n4avuu75jx5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>18gwcp5</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>How to get started with gel nails?</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18gwcp5/how_to_get_started_with_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>18gw5td</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Sally Hansen Miracle Gel | Red Eye + Deep Sea Diamond | #439 | #781</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gw5td</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>18gvton</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Did my nails for the first time!</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gvton</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>18gvkqm</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Not usually a fan of Sally Hansen but 😍😍</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/abyocdu0cx5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>18gui3q</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>I have gel x nails. Can i get them filed and refilled or do they need to be removed and i get a new set?</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18gui3q/i_have_gel_x_nails_can_i_get_them_filed_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>18gua33</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>My clean girl aesthetic nails 💅🏼 🫶🏼</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8l3vsk862x5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>18gu4ju</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>My vacation treat!!</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gu4ju</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>18gu0a1</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>I tried this German Fanta today at a food truck</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2r63sna20x5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>18gtzrf</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Christmas Sparkles ✨️</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gtzrf</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>18gtf29</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Are my nails too bulky?</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gtf29</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>18gtczm</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Kiss press ons (found at Target)! My favorite press ons yet!</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gtczm</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>18gt6e6</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Getting better but…</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gt6e6</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>18gt3uc</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Let It Snow Nails</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gt3uc</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>18gt3dv</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Did my sisters nails♥️🎄❄️</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gt3dv</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>18gt2fk</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>which nails fit me best?</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gt2fk</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>18gt0t9</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>my dream nails!!!!!</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/egzgwtqosw5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>18gswnc</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>DIY Nails, best "healthy" nail polish?</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18gswnc/diy_nails_best_healthy_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>18gsmrl</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>I’m getting obsessed with DIY Nails! 🥰</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/19cvd7lqpw5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>18gs4u2</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Chocolate Babka nails for Hanukkah 🍫🤎</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gs4u2</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>18grtnc</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>first ever acrylics!</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18grtnc</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>18grpdm</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Chocolate donut glaze</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qdwaq0gniw5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>18grhgc</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>This is as christmassy as I'm willing to go</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/334iulc0hw5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>18grbdy</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Christmas</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xiv8q64tfw5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>18gn5na</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>I loveeeee my new salon</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0pxzmixsjv5c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>18gmsxt</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>HO HO HO 🎅</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kfwiz5cvgv5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>18gqrwu</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>My holiday nails for the week!! 🎄my natural nails and did them myself, not too bad I think!</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gqrwu</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>18ggg3c</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Blossom Nail Oil</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18ggg3c/blossom_nail_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>18gpprm</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>My Holiday Nails!</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3fz9uojl3w5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>18gplp5</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Feeling quite festive</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c5tri7ux2w5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>18gpgue</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Christmas Nails in the tropics is pink.</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gpgue</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>18goz17</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Holiday nails are done!</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5supg86yv5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>18gouvl</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Need help deciding!</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gouvl</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>18gophm</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Simply Paink</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gophm</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>18gol1q</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>What's the shape best suited for my long bony fingers? I don't want to grow them out too long, but also don't want them to be plain and shapeless.</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ed7hnb41vv5c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>18gogzq</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Snowflake twist on sweater nails</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gogzq</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>18go56s</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Press on nails vs acetone</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18go56s/press_on_nails_vs_acetone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>18gnbtw</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Did some nail art but don’t have the correct brushes. Tips on making lines?</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gnbtw</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>18gmphw</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>So cute! When it cold-nails turn purple, and they are blue when it's warm</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gmphw</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>18glz4n</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Does blooming gel work with solid gel color?</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18glz4n/does_blooming_gel_work_with_solid_gel_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>18glmbs</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Hey!</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18glmbs/hey/</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>18gllvj</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>First ever D.I.Y nail art</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gllvj</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>18glg66</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>I don't know what they did at the salon...</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18glg66/i_dont_know_what_they_did_at_the_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>18gkw5j</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>*You can’t get more basic*</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/94812kz4zu5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>18gkgzq</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Nails are summer ready!</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ujv01qtluu5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>18ghvt6</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Some years ago I cut a nail on my ring finger too much, and since then its white part starts to grow too low comparing to normal level where it should start. Even when it grew up, the pink part won't stick back at that level, white starts too soon. Is there a way to glue these pink millimeters back?</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ghvt6</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>18gh7cy</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Hard Gel Natural Nail Overlay</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ehpp08wpt5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>18h9fee</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>What’s the most ridiculous thing you’ve ever done to save a fresh mani?</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/992e1el9yz5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>18gxhxo</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Seche Vite</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18gxhxo/seche_vite/</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>18h8xxs</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Space Cacao by Clionadh Cosmetics</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18h8xxs</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>18h8uyn</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>It's so pretty!</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18h8uyn</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>18h8r87</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Easing into Flakies</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18h8r87</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>18h89o1</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Recovering from my poor gel manicure.</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ci5hrpvjmz5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>18h7rr0</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>To Hell With Good Intentions</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18h7rr0</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>18h7jxs</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Trying to do a puzzle but can’t stop staring at my nails 🤩</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18h7jxs</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>18h7ev8</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>50 Shades of ... LILAC!! 🙄</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/TJs5SZK</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>18h6t20</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Ethereal Lacquer Starborn</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18h6t20</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>18h64zp</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>50% off Zoya Sale</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cpko4mu93z5c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>18h5ym7</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>[Paid/PR] - Rainbow party swirls getting me amped up for New Year's Eve!</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18h5ym7</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>18h51ok</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>A month’s worth of manis and reviews 💅🏻</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18h51ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>18h3i1d</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Photochromic Before &amp; After</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18h3i1d</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>18h3csa</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>A little festive sparkle</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18h3csa</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>18h3a22</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>💚💛ELF💛💚</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18h3a22</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>18h318q</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>💚💙🐸glass frog 2 🐸💙💚</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9hiywan1ly5c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>18h261s</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dead bugs and sparkles, who knew they'd make a great mani together? </t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/20u33ji8gy5c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>18gzfae</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Advice re: painting over dip manicure?</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18gzfae/advice_re_painting_over_dip_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>18gwu3o</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>This polish is way way more awesome in person. Riviera Rave by I Scream Nails</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gwu3o</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>18gwmpr</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>A bit rusty, a bit bloody and absolutely festive</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cd2dodc6kx5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>18gwew5</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>I’m warming up to browns</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gwew5</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>18gw3px</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Sally Hansen Miracle Gel | Red Eye + Deep Sea Diamond | #439 | #781</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gw3px</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>18gvti5</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>This should last a while!</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18gvti5/this_should_last_a_while/</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>18gvsj5</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>New nailies</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gvsj5</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>18gvey2</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Anyone else get one finger that always loses its polish?</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/56n0edprax5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>18gupnq</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>A Pretty Blue</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gupnq</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>18guo01</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>RIP my natural nail :(</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ygju8sj25x5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>18guncr</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Mooncat Sand Viper + 🍂🍁</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18guncr</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>18gtg3j</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Christmas ornament skittle</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qcqwsqwtvw5c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>18gtctx</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Dabbin’ Christmas!</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9c5o0b9puw5c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>18gt9yi</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Krampus vibes</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gt9yi</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>18gsqxe</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Winter nails.</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2bu0umimqw5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>18gseyh</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Confetti and peach jelly sandwich</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/li9xhcy2ow5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>18gs1w0</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Chocolate Babka nails for Hanukkah 🍫🤎</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gs1w0</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>18grkil</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Do my nails look diseased?</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eng9ymqmhw5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>18gr4bh</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>So Sparkly 😻</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mf1dflzbew5c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>18gqxa1</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>wintery, but not christmassy</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8gd1xecucw5c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>18gq6b0</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Joined a swatch collab to take more photos 🩵</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gq6b0</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>18gq1rc</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Mooncat What a brilliant nose</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/udatw69c6w5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>18gpzxg</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>OPI - Five Golden Flings</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gpzxg</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>18gppdo</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>ILNP Birefringence</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pzg47vwp3w5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>18gpa0j</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Sheer polish and thermals are growing on me</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gpa0j</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>18goklv</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>First attempt at magnetic polish</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18goklv</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>18gogv9</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Lesbian Pride Flag Attempt</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s12y73kauv5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>18go2ef</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>"Beeeee Goooood" E.T. injury turned polished moment</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18go2ef</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>18gnnbq</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Mooncat Pandemonium</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l4teomprnv5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>18gnl7m</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Starting to get festive...</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qnvweteanv5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>18gnia3</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Cozy warm set</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gnia3</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>18gmcow</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>She’s a mood</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tggobj70dv5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>18gm9a0</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Holiday nails for the win!</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gm9a0</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>18gm8ds</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>DIY Swatch Book</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gm8ds</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>18gjioz</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Can I cut newly lacquered nails?</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18gjioz/can_i_cut_newly_lacquered_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>18hbxyk</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Blue Cat Eyes</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hbxyk</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>18h9wsq</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Viral Eyeshadow Makeup Trend BUT FOR NAILS?!</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18h9wsq</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>18h8tg6</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Xmas nails</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18h8tg6</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>18h8svb</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Xmas nails</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jc0nawhtrz5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>18h6hdt</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Spooky Set ✧</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mnfhrlw36z5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>18gyqo0</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Opinions? Honest advice?</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p1in7twmxx5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>18gyoji</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Opinions? Honest advice?</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3mlparvbxx5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>18gyn07</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Opinions? Honest advice?</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yt7f87d3xx5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>18gyly1</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Opinions? Honest advice?</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6fyp0rdxwx5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>18gykjl</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Opinions? Honest advice?</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y7wimidpwx5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>18gyjwl</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Opinions? Honest advice?</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0958ldrlwx5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>18gwhb0</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>My nails last week as a nail tech. Gingerbread and GirlyPop Christmas! Done by me Jolley.nails</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gwhb0</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>18guyje</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>It’s the holiday season</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18guyje</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>18guxw4</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Nail polish, base coat or gel or anything else?</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/18guxw4/nail_polish_base_coat_or_gel_or_anything_else/</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>18grc6i</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Christmas</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q1ext76yfw5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>18gq1mk</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>❄️ winter vibes</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18gq1mk</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>18goq0t</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Holiday Glitter</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rzbsa3f9wv5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Dec 14 08:08:18 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_12_17.xlsx
+++ b/data/2023_12_17.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C614"/>
+  <dimension ref="A1:C765"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10871,6 +10871,2573 @@
         </is>
       </c>
     </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>18i3nt6</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>My friend called them fruit loop nails</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fxsy345fv76c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>18i2wm8</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>hello! i was asked to post some more nail art (literally one person lol)</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18i2wm8</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>18i2k9q</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>My first gel nail polish done by professional</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4el7ulkoh76c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>18i29sr</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Does it mean anything to have translucent nail tips?</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18i29sr/does_it_mean_anything_to_have_translucent_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>18i27jo</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>a subtle santa moment</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18i27jo</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>18i1no7</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>hi! i’ve been doing my own gel-x nails for a while, what do you guys think? any suggestions or tips?</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18i1no7</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>18i1bfp</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Copy paste 📝</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18i1bfp</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>18i12je</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Nailfies</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18i12je</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>18i0ufy</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>An old set I did for my friend as part of her bday gift</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18i0ufy</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>18i0pcn</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Before and after</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18i0pcn</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>18i07lc</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Winter nails!</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18i07lc</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>18i02vn</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>I've done my own Christmas nails 💅🎄</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ec984lwzq66c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>18hzwph</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Which nail shape for large hands?</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pcpd574ap66c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>18hz38y</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>What glue works best for false nails?</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/55ilp0obh66c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>18hywls</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>I've never done any nail art before, have any tips?</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hywls</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>18hyphs</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Cuticle bits?</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18hyphs/cuticle_bits/</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>18hydsq</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>I’m getting close up pics with my husband and toddler. Would you go back?</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hydsq</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>18hy7eg</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>My first press on set!</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jwngx0l5966c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>18hy66j</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Can acrylics last four weeks? Usually do dip for a four month set.</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18hy66j/can_acrylics_last_four_weeks_usually_do_dip_for_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>18hx8kk</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>I’ve enjoyed pressons and changing them frequently. I’ve gotten a lot of compliments, what do you think?</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vgpl71ob066c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>18hx44r</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Love my new xmas nails!</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/75nk1lb7z56c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>18hx2sc</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Death Valley Nails - Dill Weed</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hx2sc</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>18htny8</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>My favorite manicure ever</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18htny8</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>18hro9h</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Wintery nails</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/stqjwvc2r46c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>18hro6f</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>The mani 💅🏻 ➡️ the inspiration 🎄</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hro6f</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>18hwiyk</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Junji Ito nails i did on my sister for halloween! (i know it’s been a while since then but i’ve always been nervous to post my work)</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/umsn2upyt56c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>18hwhld</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>pastel space nails ✨</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8rkcimkmt56c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>18hweas</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>What color nails for a wedding in this outfit?</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p47hqvfws56c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>18hwa4r</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>I ❤️💚 Christmas by me. I think I found my perfect nude!</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hwa4r</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>18hvw30</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Christmas Nails 🎄</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j39kpw0io56c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>18hvt1d</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Tortoiseshell and turquoise</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/upvwtqxqn56c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>18hvjxq</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Favorite vibrant vinyls scent?</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18hvjxq/favorite_vibrant_vinyls_scent/</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>18hue06</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>They are simple, but I love daisies ♥️🌼</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sfvmdhxyb56c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>18hu854</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Holiday nails</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/67ls32vma56c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>18hu40p</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Love this color</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mwl4f52q956c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>18hscvl</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>(Acrylics) nude Xmas nails vs inspo by @nailyuuuu</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hscvl</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>18ht7fg</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Cuticle care cream</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ht7fg</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>18ht5d1</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Oily nail beds?</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18ht5d1/oily_nail_beds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>18ht07v</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Nail Community help me blow my girlfriend away</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18ht07v/nail_community_help_me_blow_my_girlfriend_away/</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>18hrutc</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>essie fairy tailor ✨🧚‍♀️</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hrutc</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>18hrp00</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Simple yet pretty gel for christmas❤️</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m7ijtbs7r46c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>18hrdli</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>What are some good affordable airbrushes for nails?</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18hrdli/what_are_some_good_affordable_airbrushes_for_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>18hr879</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Acrylic Nail Question!</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18hr879/acrylic_nail_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>18hr60q</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Can i make press on nails with gel x tips?</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18hr60q/can_i_make_press_on_nails_with_gel_x_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>18hqwzd</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>dyeing acrylgel or builder gel?</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18hqwzd/dyeing_acrylgel_or_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>18hqj49</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Before and after</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hqj49</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>18hqeqj</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>What are good winter/xmas nails beside green or red?</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18hqeqj/what_are_good_winterxmas_nails_beside_green_or_red/</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>18hoojz</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>It's giving runway</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hoojz</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>18hqbth</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Ready for Christmas! My natural nails are flourishing 🥹</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ktl0ebxmg46c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>18hq5ks</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Merry octomas and happy hollydays!</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/86z2xgsaf46c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>18hpq1c</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>dip powder manicure question</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18hpq1c/dip_powder_manicure_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>18hpagk</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Nails color recommendations for someone with neutral warm undertones?</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18hpagk/nails_color_recommendations_for_someone_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>18hpaa7</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Second set I’ve done so far</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yntrwxhl846c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>18hp62o</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Pre-Christmas nails…</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pkmwhptq746c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>18ho7s4</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Hard Gel vs Acrylic Overlay vs Dip</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18ho7s4/hard_gel_vs_acrylic_overlay_vs_dip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>18hokr7</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Good almond full cover gel tips ?</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18hokr7/good_almond_full_cover_gel_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>18hoc0z</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Christmas Nails!</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yqpg71jb146c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>18hobad</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Red cats eye</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hobad</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>18hnela</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Some of my milky white nails this year</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hnela</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>18hn78l</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Attempt at french manicure</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hn78l</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>18hn0p1</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Sculpted gel nails</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yfeqb2bcr36c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>18hmw1m</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Is it okay to ask for an estimate before booking an appointment with a nail tech?</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18hmw1m/is_it_okay_to_ask_for_an_estimate_before_booking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>18hmrdj</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Obsessed with my lilac</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hmrdj</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>18hme23</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Christmas set 🎄❄️ all hand sculpted 😍💗</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hme23</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>18hmbbh</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Christmas and birthday all in the same month…I just had to match my nails.</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sfka6m94m36c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>18hm39a</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Winter nails. did them by myself 🥰</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ntoozy4hk36c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>18hlzny</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>It's beginning to look a lot like Christmas - New set</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hlzny</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>18hjede</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>I love my new nails, but how do you deal with the rough surface of the glitter? It's catching on everything</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/inwb8zzrz26c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>18him09</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>1 year of gel manis</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18him09</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>18hij93</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Hanukkah nails inspired by the black &amp; white cookie 🖤🤍</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hij93</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>18hhitz</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Polygel nails keep breaking less than 24hrs after being done</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18hhitz/polygel_nails_keep_breaking_less_than_24hrs_after/</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>18hlres</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Ice ice baby 🧊❄️</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hlres</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>18hl5h5</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Flower power</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7kzemqzkd36c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>18hkl68</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>I don’t get my nails done very often - should the corners of the gel polish be lifting after only 5 days?</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r6u88po8936c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>18hjxfn</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Chill set by me</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hjxfn</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>18hjldi</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>First time chrome frenchies</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2qh2uy9a136c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>18hjfb2</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Christmas sweater weather</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hjfb2</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>18hiw5d</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Simple stars ✨</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hiw5d</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>18hingq</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Longest my natural nails have ever been! I painted these cute little bows on them and I love.</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/77zmmbupt26c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>18hifte</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Happy holidays</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5dnkf8nyr26c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>18hhtn9</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>holiday set :)</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hhtn9</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>18hhsel</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>We went for a celestial vibe, added a heart because I’m a bridesmaid this weekend 🖤✨</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3m10322km26c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>18hh9tc</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Chrome Acrylics!</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yaajqy62i26c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>18hh8wi</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>🪩</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gm9gv2gth26c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>18hggnj</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Christmas Nails 🎄</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hggnj</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>18hg1v1</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Ready for christmas. 🎄❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k6fsuwv9626c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>18hfned</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>These polka dots are nothing compared to some of the gorgeous art on here, but it's my first time doing something like this and I thought I would share it! Anybody have any easy designs I can try out next?</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3310kjq4226c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>18heafm</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>My practice set!</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d9ibtwtjm16c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>18he717</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Nails in Munich, Germany</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18he717/nails_in_munich_germany/</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>18he0zh</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>From gel to polish 💅 Although my nails are always protected when doing gel nails, I do like to cut my nails and use polish instead once in a while. I feel like my nails need a break from all the gels, they can regenerate and get harder after that. Do you do that as well?</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgute038j16c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>18hdpb9</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Season for Christmas nails 🎄</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hdpb9</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>18hdhvu</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>will acetone-free remover mess up gel?</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18hdhvu/will_acetonefree_remover_mess_up_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>18hdenl</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Obsessed. I’ve been wanting red frenchies for a min but didn’t have the time to do them. I had done a pink nude 2 weeks ago and wanted to extend the life of them so I just added the red. I love it, even though it’s not perfect!</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hdenl</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>18hd3tl</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>OPI Salty Sweet Nothings vs Essie Birthday Girl</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rlmwpcqg716c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>18hcp0z</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>In mourning</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2yb4r5dx116c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>18hc21b</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>My wedding nails. The best nails I've ever had</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8y297ggct06c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>18i34df</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>🐰Mooncat’s Wish I Hadn’t Cried So Much🐰</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rx2fswdgo76c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>18i1iyc</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>First Pick of my ILNP Black Friday Haul!</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18i1iyc</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>18i1hdk</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Trying out magnetic toppers!</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qxvww04j576c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>18i0ftb</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Moonshake by Clionadh Cosmetics</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18i0ftb</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>18i0c83</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nail tech always knocks it out of the park: duo duochrome velvet nails </t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vkr8oxgkt66c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>18hznoq</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>wanted to share my first mani of December</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b4q2amqrm66c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>18hz91g</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Weird change I. Texture with top coat</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4rj1m06vi66c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>18hz54f</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Unknown Wintery Polish</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hz54f</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>18hybx5</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Clionadh ‘Psilocybin’ with a ring magnet</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nw98xzr9a66c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>18hy5u6</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Tortoiseshell Nails 💛❤️🤎🖤✨</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hy5u6</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>18hy3gx</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Leslie - Zoya 💜</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hy3gx</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>18hxjpr</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>I never thought I'd be a flamingo pink lady, but here I am!</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hxjpr</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>18hx4n0</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Death Valley Nails - Dill Weed</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hx4n0</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>18hwhgw</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Thinner top</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/te7b29clt56c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>18hwbt2</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>I ❤️💚 Christmas by me. I think I found my perfect nude!</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hwbt2</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>18huvij</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Orly - Let The Good Times Roll</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18huvij</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>18hs7tt</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Claus it's the most wine-derful time of year</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5pjpbgd6v46c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>18hrsy8</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>SPOILER: Lūmen stained glass mysteries revealed (complete menagerie)</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hrsy8</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>18hr0na</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Christmas lights</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qm6stw20m46c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>18hos21</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Winter Grays</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hos21</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>18hpy58</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>I’m getting gel extensions for the first time. What can I expect?</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18hpy58/im_getting_gel_extensions_for_the_first_time_what/</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>18hq6dv</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>My christkindlmarket nails ft mooncat your heart is a black hole and mooncat I’m a mf supernova.</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d1590hahf46c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>18hpe0k</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>I love this $2.50 Zoya red.</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mn3gmcre946c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>18hp5s5</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>PSA Baking Lacqueristas: Topcoat can melt 🥵</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jfnh0mco746c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>18ho0b5</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>First neon and I’m SOLD</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ho0b5</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>18hn8fu</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Cadillacquer Kiss Me (November Polish Pickup)</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x5kyidrxs36c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>18holit</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Coquette 🎀</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18holit</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>18hoige</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Vampire Vibes 🩸</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hoige</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>18hoh5h</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Glitter Bomb 💣</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nrbkcs8f246c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>18hnnir</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>I am not allowed to put the nail polish away</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pzp6q7d0w36c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>18hn66m</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>How do you organize your polish? By color, brand, collection, finish?</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18hn66m/how_do_you_organize_your_polish_by_color_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>18hmmg4</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Classic for a reason</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pssulj8fo36c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>18hlxyp</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Ghost polish recs?</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hlxyp</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>18hloe9</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>BKL Shipping?</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18hloe9/bkl_shipping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>18hl2cj</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>BKL Immortality is a STUNNER</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hl2cj</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>18hkkd3</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Pyro but make it Christmas</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hkkd3</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>18hjnab</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>I don’t know how you all take such beautiful photos, but here’s my holiday addition!</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hjnab</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>18hjka5</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Christmas sweater weather</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hjka5</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>18hik3s</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>(PR) Hanukkah nails inspired by the black &amp; white cookie 🖤🤍</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hik3s</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>18hicrq</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Bluuuuueeeeeee</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3gd92tt9r26c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>18hi8q5</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>new polish over few days old mani?</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18hi8q5/new_polish_over_few_days_old_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>18hgwq6</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Any way to whiten nails that actually works?</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3166m0dqe26c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>18hgr6k</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Cuticula, where are you now?</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18hgr6k/cuticula_where_are_you_now/</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>18hef4a</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>How long should I wait to paint my nails after showering?</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18hef4a/how_long_should_i_wait_to_paint_my_nails_after/</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>18he6yb</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Super chuffed with my Chrismassy press ons 🥹</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18he6yb</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>18hzoqi</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>New to designs. Still adjusting to “look at me” nails. Haha</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hzoqi</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>18hyvht</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Xmas time me night Mani (at home always)</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/92wp8vf9f66c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>18hy6yy</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first press on set </t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g9buz741966c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>18hx1ud</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Tis the season 🎄❄️</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ve6kkpqly56c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>18hwcj9</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>I ❤️💚 Christmas by me</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hwcj9</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>18hu5fu</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Nails I did in myself yesterday!</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18hu5fu</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>18hlw9w</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>When your gf is a gamer and wants her nails done</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7r6qda71j36c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>18hfosq</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>My first nails done by my friend from class, what do you think?</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fn7efnkk226c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>18hc2kb</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Millennial Hotties</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ms7icejxs06c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>18hbzqa</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>My first post press-on nails</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/aa6ugmk9s06c1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Dec 15 08:08:14 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_12_17.xlsx
+++ b/data/2023_12_17.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C765"/>
+  <dimension ref="A1:C954"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13438,6 +13438,3219 @@
         </is>
       </c>
     </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>18iv5a0</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>I’m so happy</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/30s61geh1f6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>18iudgs</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Alternatives for acrylic</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9auqa0vsre6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>18itvjq</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Today I F***Ed Up Nail Edition</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bvk4v7a0me6c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>18itp3l</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Death valley nails 💜</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cw462epwje6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>18itozr</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Just my sparkly purple nails</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/co2xqofvje6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>18itcya</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Is there too much space between my gel and cuticles? Got these done yesterday and it's been bugging me 🥲</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18itcya</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>18it9sw</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>was supposed to get something slightly different:’)</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w56pcz16fe6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>18isfhw</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Need Advice: Storing nail polish in a cross-country move?</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18isfhw/need_advice_storing_nail_polish_in_a_crosscountry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>18is93k</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>My press ons match this gift bag!</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wfbfuwh74e6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>18irr6y</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Update for the haters: Death Valley Nails - Dill Weed as a topper</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18irr6y</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>18irqrs</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Update: Are my nails too bulky?</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18irqrs</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>18irohb</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>the opalescent effect is not totally captured but it’s so pretty irl</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18irohb</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>18ir1n4</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>How Can I Make Red And White Candy Cane/Peppermint Nails?</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18ir1n4/how_can_i_make_red_and_white_candy_canepeppermint/</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>18iqu3t</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Glamnetic or suggestions?</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18iqu3t/glamnetic_or_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>18iq17e</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Christmas press on nails</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18iq17e</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>18ipzlk</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ipzlk</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>18ipxof</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Is this weird or no</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18ipxof/is_this_weird_or_no/</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>18ipkv0</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Playing with lines!</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ipkv0</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>18ipkl6</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>14/12/2023: Trying out a different shape, so far I’m liking it a lot. Opinions?</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ipkl6</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>18ipj2f</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>This weeks nails, trying long almond shape</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ipj2f</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>18ipdu2</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Christmas nails! 🐻‍❄️🎄❄️</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/226s6i1acd6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>18ioszq</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Today I chose this model ✨</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/klpckyfw6d6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>18ioggs</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Absolutely in love with this Christmas set 😍</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ioggs</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>18iocmb</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Did my mom’s nails 🥰 Please roast them and help me get better💪</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r1gnfuls2d6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>18iobto</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>a color so heinous it’s cute</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18iobto</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>18inct8</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Blue Christmas nails</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18inct8</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>18in7tn</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Winter wonderland 🎄❄️</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z29csuqlsc6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>18in43f</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>before vs. after</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18in43f</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>18imgqd</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>First time trying magnetic polish!</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/80kbp8o8mc6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>18ilsui</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Christmas nails! 🎄❤️</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jqc4d9logc6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>18ilsbj</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>I love them 😍</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ilsbj</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>18ii1fh</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Nail Troubleshooting</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ii1fh</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>18ilcly</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Simple ✨🩵</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0p9ndz10dc6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>18ikx9g</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>New set today for Christmas!!!!!</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0amiiunq9c6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>18ikr8e</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Snowflake nails for winter ❄️ 🥶</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3uvnok5f8c6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>18ikj6y</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>These are the best set I've done so far. I'm so proud and need to show someone!</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e8u2u6to6c6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>18ikfy6</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Winter date</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ikfy6</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>18ik4ex</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Porcelain nails?</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18ik4ex/porcelain_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>18ijz5q</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Received spilled Mooncat</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ijz5q</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>18ijyci</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>3 months of growth down the drain</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ijyci</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>18ijpgd</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Anyone knows how this style is called so I can replicate it with gel?</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dywy6dm90c6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>18ijg89</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Christmas time!</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z2hql7w8yb6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>18ijeu8</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>What’s the best shape for my nail beds?</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ijeu8</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>18ij5ua</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Difference in lifting depending on Gel X shape?</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ij5ua</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>18ij3tt</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>3xl press ons</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1we99fxhvb6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>18ij17w</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Nail care tips</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uj0kzkxvub6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>18iiwn7</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>christmas nails</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9fmff0cvtb6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>18iirg5</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>I was trying to do flowers but ended up doing eggs instead</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lvgylaposb6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>18iiqhx</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>I’m so happy with how these came out! All hand painted by me</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ncy252hsb6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>18iigd0</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>super shimming nails this time :)</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18iigd0</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>18iibvp</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Love my fresh set 🔮🦄🛸</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18iibvp</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>18ii6cl</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Reverse French Christmas nails 🎄</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/arglzr41ob6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>18ihwxm</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Feeling festive with a sparkly ombré tip ✨</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/23ugw0lylb6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>18ihtpa</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>New Set</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ihtpa</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>18ihk3k</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>❤️ Just a ✨ hint ✨ of Xmas 💚 Painted Polish Let It Dough from their Christmas collection a couple years ago</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ihk3k</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>18ihh22</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Red under acrylic nail growth? Btw this is fake stuff prob. Chop shop. It’s been almost a month of no fill bc I’m going to a new independent nail tech and need to remove them myself first but am on vacation. Is it bc they’re too overgrown? Should I cut? feels fine It just happened today</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/68omrg9iib6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>18ihgvu</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ihgvu</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>18ih379</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>A set I had from this past summer</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5aexfxgfb6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>18igyze</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Elegant Holiday Nails!!</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nthvc2mieb6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>18igehm</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Christmas mani diy</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18igehm</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>18ig1lv</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Witchy</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ljhkfu637b6c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>18ifzlz</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Balletcore nails 🩰</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ifzlz</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>18ifrzv</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>I was so in love with these Halloween nails!</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y0jwezpy4b6c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>18ifovo</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Slightly Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ifovo</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>18ifa69</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>🎄christmas nails✨</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3wq5xnb01b6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>18iezlc</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Im in love</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3svoou2oya6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>18ierb8</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>I love them and you?</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gagur36wwa6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>18iebjp</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>How do we feel about the reverse frenchie?</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iopojgukta6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>18ie9xv</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>I did my Christmas nails</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fwcazvx8ta6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>18idsug</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Gel x nails</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8jce7tgjpa6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>18idpj8</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>I tried French tip on my girlfriend. I've never done this before. Learned a lot.</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gipzey7uoa6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>18idhpf</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>got my christmas nails today ❤️🎄💚.</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/49lr7o05na6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>18icv8w</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Help with peeling nail beds</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zpyg1sr8ia6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>18icwzq</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>one of my fav sets so far 🥰</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18icwzq</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>18icwxt</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>first set on myself that i’m proud of !</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18icwxt</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>18icghk</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>My "gaudy 90s decorations" inspired Christmas nails! On me by me 🎄</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18icghk</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>18ic6p3</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Gingerbread</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/agqjcyprca6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>18ic2yh</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Baby pink gel nails with a small glitter accent on myself by me!!!</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/am20howwba6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>18ibzx6</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>I did my nails myself for the first time</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o7jhafa9ba6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>18ibyww</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q6pmp7m0ba6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>18ibvd8</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>How are my holiday nails?</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ibvd8</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>18ibnl1</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>my Christmas nails❄️❤️</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7uyyl70h8a6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>18ibm07</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Love a good random match of colors!</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vupyf2k38a6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>18ibcaz</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Hanukkah meets Mooncat 🪬🪩🩶🧿</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ibcaz</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>18ib4eg</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Christmas nails done by me 🎄</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c0rrzn404a6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>18i8lkf</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Holliday inspo 💚</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o71pvmaci96c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>18iawa3</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Thoughts on these nails</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0e3id0942a6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>18iahpw</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Does this red look good with my skin tone ? I usually only get nude colors.</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k0xuhznvy96c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>18iahpq</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e9n3r5dvy96c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>18iabh7</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Classic but cute</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f54b7peex96c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>18i9uyp</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>It’s beginning to look a lot like Christmas</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wjnuhxzjt96c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>18i9cv7</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>second gel extension set ive done, i think ive improved slightly</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bshwz497p96c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>18i8lmv</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Snowy and sparkly for Yule</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cfy42asci96c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>18i8eal</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Press on nail help</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18i8eal/press_on_nail_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>18i31zf</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>i didn’t want to make separate posts for all of them so here are most of the ones that i’ve done this year:)</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18i31zf</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>18i4o0a</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Is my nail lifting or is the gel-x tip lifting?</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18i4o0a</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>18i6g64</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Nude,pink and dipped glitter</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0rv3hhr4v86c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>18i5z0p</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>❤️🧑🏻‍🎄Christmas Nails 🧑🏻‍🎄❤️</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2nypalmcp86c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>18i5tj7</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Builder Gel+Texture+Chrome</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18i5tj7</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>18i4f5k</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Purple Kuromi Nails 💜</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18i4f5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>18iteqp</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>First set of acrylics in years &amp; I’m pretty satisfied!</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18iteqp</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>18itddk</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Help me pick my Xmas color!</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18itddk</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>18isqbu</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>first velvet attempt... fail?</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nwyt3ix69e6c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>18ise76</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Candy Canes</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jhdryxqj5e6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>18iro82</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Update for the haters: Death Valley Nails - Dill Weed as a topper</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18iro82</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>18ir3v6</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Bought this when I couldn’t get Coronation</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ir3v6</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>18ir32c</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Some nearly neon red and green. If I can’t literally BE Christmas lights, I’m gonna look as close to them as I can. 😂</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ir32c</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>18iqxfd</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Kitschy sugarplum skittle</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18iqxfd</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>18iqq9g</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Picked this color specifically because it reminded me of the Northern Lights</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j82yjlgwod6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>18iq4hn</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Expert Opinion</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m9s4sk58jd6c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>18ipmyz</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Holo Taco - Everything Is Pine</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ipmyz</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>18iaqx1</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Issues with Gel - top coat feels like it doesnt cure all the way? Smudges and doesn't feel hard.</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pvmxkwtu0a6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>18iep51</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Looking for a sheer but good coverage just like this one in the picture - ideally polygel from Amazon or gel color</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i0cfjzrfwa6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>18ip889</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Looking for help from the crafty nail art people here.</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ip889</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>18ioqc2</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Fake Halo after 9 (!) days of wear!</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ioqc2</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>18io61i</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>ILNP Party Bus vs. Cityscape</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18io61i/ilnp_party_bus_vs_cityscape/</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>18io4q4</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>i’m finally feeling Christmasy♥️💚</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18io4q4</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>18injhr</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>coronation 👑💜</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o5nzrthgvc6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>18ind7t</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>has this happened to anyone else with china glaze?!?</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hi4epy9xtc6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>18imwua</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Any Thoughts on LA Colors Quick Color?</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oa4b3spypc6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>18imrs8</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Cuticle help?</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o83uo5isoc6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>18imqea</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Magnetic toppers? (Looking for similar ideas to Cirque's 'Chemistry')</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18imqea/magnetic_toppers_looking_for_similar_ideas_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>18imp8m</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>How to manicure peeling nails?</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18imp8m/how_to_manicure_peeling_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>18ilz9k</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Fake Essie gel couture?</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ilz9k</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>18il5y5</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Last week's winter manicure (+ bonus cats)</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18il5y5</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>18il3cy</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Holiday Nails!</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18il3cy</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>18ikoq1</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Sleepy Holo (Trypophobia?)</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ikoq1</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>18iklm3</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Christmas is Carnage on Shorties</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18iklm3</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>18ikhs4</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Best Brand for Magnetic Polish??</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18ikhs4/best_brand_for_magnetic_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>18ikfvb</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>It doesn't feel like Christmas but figured I could still do themed nails 🎄</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e2703s6y5c6c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>18iiu81</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>BKL - Secrets</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18iiu81</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>18iifzi</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Chaotic Christmas skittle 🎄💅</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18iifzi</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>18ihtj4</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Plum Pudding</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ihtj4</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>18ihid9</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>❤️ Just a ✨ hint ✨ of Xmas 💚 Painted Polish Let It Dough from their Christmas collection a couple years ago</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ihid9</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>18ih6d6</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Any tips for a cleaner finish?</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/396gnem6gb6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>18igpyg</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>searching for a great black-red</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18igpyg/searching_for_a_great_blackred/</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>18igmpv</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>A little holiday cheer</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yrcodmrtbb6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>18igj3r</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Orly Pine-ing For You</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h3m9r6o0bb6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>18ifzqd</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Quest for the Perfect Peacock</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ifzqd</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>18iflxu</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Icy, but fabulous fingers.</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18iflxu</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>18iessi</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Lord Leighton and The Wizard - A England</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cdkq0lk7xa6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>18iems0</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Unsure about Hidden Potential</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18iems0</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>18ie248</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>High key obsessed with “Your Heart’s a Black Hole” velvetized</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5rhr0d1jra6c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>18idvzx</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Gel dupes for Holo Taco and Mooncat?</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.holotaco.com/products/sacrificial-lacquer</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>18idni1</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Cirque Coronation Comparisons</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18idni1</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>18idn8w</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Can't get builder gel to stick</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18idn8w/cant_get_builder_gel_to_stick/</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>18idh6i</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>‘Tis the Damn Season</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ngcv1fl0na6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>18idb59</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>officially in love with the color brown 🤎</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18idb59</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>18id9o6</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Hi little gingerbread man!</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/94j1x5gcla6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>18id2zm</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>She’s a beaut 😍</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18id2zm</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>18icwep</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Pls help me with choosing a cute elegant nails</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18icwep/pls_help_me_with_choosing_a_cute_elegant_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>18i8wqv</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>ILNP - Sandbar</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18i8wqv</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>18ibmc3</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Love a good random match of colors!</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nrb3v0e68a6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>18iba7z</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>❤️🤍Candy Swirls🤍❤️</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18iba7z</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>18ib1rl</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Another velvet hack</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/twculbhb3a6c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>18iax00</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Hanukkah meets Mooncat 🪬🪩🩶🧿</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18iax00</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>18iasth</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Yucca in Bloom</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b17ibipa1a6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>18iaquf</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>1968 Sue Preé Fantasy Glitter</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bq1tivou0a6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>18ia44j</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>ILNP VIP</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8gwvtvvmv96c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>18i9pzg</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>{PR} After Hours by ILNP 💕</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/90n1v7yfs96c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>18i9lj2</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>I’m always drawn to the ‘weird’ polishes in new releases</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18i9lj2</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>18i95ug</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Finally created the table I had planned</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18i95ug</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>18i83ht</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>One of my all-time favorite polishes for my birthday/Christmas nails! ❄️</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sea1iened96c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>18i7slw</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Snow Globe Nails</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18i7slw</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>18i789n</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Do you also have nail polish stains everywhere in places where they don’t actually belong?</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ruuza3x396c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>18i641y</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Essie sheer polishes not drying</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18i641y/essie_sheer_polishes_not_drying/</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>18i5qzg</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Tried some new drugstore nailpolishes. Love this one</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/opv2rcfmm86c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>18i49j9</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Redemption for death valley nails after the dill post?</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8b2bddz6386c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>18isfcc</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Vacation Vibes My Godmother's Stunning Nail Art Unveiled by a Stand-In Nail Tech!</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://imgur.com/mT5oTek.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>18ir75f</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Pink Vintage Christmas</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ir75f</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>18ipx62</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Holiday nails I did myself.</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ipx62</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>18ipltv</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>3d nail art</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ipltv</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>18ipjrr</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Playing with lines</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ipjrr</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>18ip5i8</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Winter Nails</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/obmab7n5ad6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>18ip126</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Christmas Confetti ✨ all handpainted</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ip126</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>18imlfl</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>I went hyper-speed and did these in 90 minutes before an outing the other day 😮‍💨 They're pretty rough, but I'm happy with 'em 🥰</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18imlfl</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>18imb9e</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>A twist on the classic French!</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18imb9e</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>18ilumr</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Christmas nails! 🎄❤️</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e23zgzq3hc6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>18il14z</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Would you just look at em?? And of course the handsome background boy</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18il14z</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>18ikc9z</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Winter date</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ikc9z</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>18ijx8p</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>melokuro set 🖤🎀</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ijx8p</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>18iivth</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>christmas nails</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hht8glyotb6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>18ihlj5</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>My best friend is a nail tech</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o1hm0ochjb6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>18ih7to</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>We all like fires 😍😍</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nnma35nhgb6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>18iftdd</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>DIY Gingerbread House Nails!</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g15tgby95b6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>18iebv4</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>pastel space nails ✨</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s60lov7nta6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>18ie2pz</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Christmas nails ❄️🎄</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/irzl2smnra6c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>18i7v9n</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Snow Globe Nails</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18i7v9n</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>18i6gey</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>New set!!</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9qd7e418v86c1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Dec 16 08:07:15 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_12_17.xlsx
+++ b/data/2023_12_17.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C954"/>
+  <dimension ref="A1:C1103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16651,6 +16651,2539 @@
         </is>
       </c>
     </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>18jm8g6</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18jm8g6/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>18jlaa0</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>My nail tech is my bestie</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/95ujsdrarl6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>18jkdbk</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>I feel this in my bones lol.</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j4d1u4kvgl6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>18jk2v7</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>You guys she butchered my nails :(((((</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2mo8f79qdl6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>18jjfgb</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>reflective glitter with holly for christmas!! gel x done on myself!!</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jjfgb</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>18jilvr</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Grapefruit sparkle gel</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jilvr</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>18jjtcj</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Got my very first mani/pedi today, and I'm in LOVE!</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jjtcj</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>18jjnil</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Holiday Vacay x Disney Nails</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jo7it5089l6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>18jjn58</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>First time trying sparkly gel</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rrsut3949l6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>18jiotm</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>My first French tips</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jiotm</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>18jin4l</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Gel X Removal</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18jin4l/gel_x_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>18jihap</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Did my mom's holiday nails!</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jihap</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>18ji7jy</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>How’s the cat-eye effect on these?</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/23fmq5vluk6c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>18ji50a</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>One of my favorite colors forever! Any Christmas recommendations? Red is not an option☺️</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rox5fn0wtk6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>18jhdd4</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Going to Christmas dinner this weekend. Just a simple glitter but SO cute 😊</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mezn8wyamk6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>18jgzy4</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Christmas nails 🎄</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jgzy4</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>18jgxy7</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Press ons</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jgxy7</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>18jgq3b</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Holiday red nails ♥️</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h5nj0hh3gk6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>18jd7n7</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Feeling fancy with my beige airbrushed tips</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l0lrdp3mkj6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>18jgcvx</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Any recommendations for fast drying nail polish?</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18jgcvx/any_recommendations_for_fast_drying_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>18jgaa6</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Advice needed!!!!</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jgaa6</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>18jg7cy</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Red Christmas nails</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jg7cy</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>18jfw7g</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Natural nail with gel polish🥹</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8xywglv28k6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>18jfd30</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>gel x</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18jfd30/gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>18jezij</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Do you guys prefer sticky tabs or glue? I used sticky tabs here, but I don’t really like how it’s not flush with the nail and my hair gets stuck in it</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jezij</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>18jek1g</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Reflective ones ❤️</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hy1w06x2wj6c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>18jeawx</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Holiday Nails</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jeawx</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>18je5xt</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Types of Gel</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18je5xt/types_of_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>18je2u6</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Following the North Star</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18je2u6</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>18jdkx7</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Bio gel or shellac nails?</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18jdkx7/bio_gel_or_shellac_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>18jd8ad</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Can I cut my gel extension nails</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18jd8ad/can_i_cut_my_gel_extension_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>18jcz8b</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>My favorite Christmas set ever 🎄</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jcz8b</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>18jcxio</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Red velvet for Christmas ❣️</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jcxio</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>18jctjw</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Christmas set by me! 🎄</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jctjw</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>18jcq5i</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>New design</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mj2s6xdpgj6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>18jc0gp</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>What is going with the orange streak in my nail?</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/71uopwgwaj6c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>18jbyg5</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Kiss Impress Classic French</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fzvhak9gaj6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>18j7qpw</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Advice wanted</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18j7qpw</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>18jbgwa</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Constant skin and nail biting</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jbgwa</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>18ja912</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>It has been a pink Christmas this season</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/73w5fafvwi6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>18j9r65</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Do these look like press ons?</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18j9r65</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>18j9dy1</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Christmas gel x nails that took me way too long 🤍</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wig9d1svpi6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>18j98pc</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Growth on short nail beds</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zn2sc94ooi6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>18j8w5v</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lfk2t04wli6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>18j8kj7</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Holiday Depression nails 🤧</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18j8kj7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>18j8g0w</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xz6u1q49ii6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>18j88yp</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Holiday set, I'm very much in love!</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gz9htl8ogi6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>18j7tdt</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>starting over fresh. 💅✨</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18j7tdt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>18j7lss</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18j7lss</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>18j6qat</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Are these nails too long for my finger length?</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18j6qat</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>18j6aid</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Should I paint all nails glitter or keep the baby pink?</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18j6aid</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>18j52mx</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Xmas nails!</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18j52mx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>18j4zpr</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>which nail shape would you recommend for me?</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6qnsys9erh6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>18j4r2s</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Latest manicure</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/of9kmjhiph6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>18j4mbv</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>First time trying dip, first time with this nail shape, and first time trying French ombré. I think I’m in love! [Salon-done]</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18j4mbv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>18j3clu</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Seeking advice: hiding nail flaws</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18j3clu/seeking_advice_hiding_nail_flaws/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>18j3vdc</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Christmas nails (again)</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18j3vdc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>18j3q3l</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Chrimbo nails.</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18j3q3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>18j3n67</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Membership based salon. Is it worth it for $135/month?</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.glosslab.com/book-services?locations=south-miami%2Csunset-harbour%2Ccoconut-grove&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_adgroup=%7BAdGroupName%7D&amp;utm_term=glosslab&amp;utm_campaign=%7BCampaignName%7D&amp;utm_source=google&amp;utm_medium=cpc&amp;hsa_acc=2121624743&amp;hsa_cam=17880762404&amp;hsa_grp=152063926238&amp;hsa_ad=665604890399&amp;hsa_src=g&amp;hsa_tgt=kwd-381281974936&amp;hsa_kw=glosslab&amp;hsa_mt=p&amp;hsa_net=adwords&amp;hsa_ver=3&amp;gclid=Cj0KCQiAj_CrBhD-ARIsAIiMxT_ZbgjuCocfovUyQyZtYmQkG_P5K53BjO3T2JR4wVCUTpI8AAnG75saAh-LEALw_wcB</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>18j35l6</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Pre Christmas nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hm4nd0wwch6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>18j2dpb</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Pink medium length almond nails 💕</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/od8epd1q6h6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>18j1qqq</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Christmas nails ☃️</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sb4muwuj1h6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>18j18gb</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>If you experience lifting with soft gel tips even after fully preparing your nails... Do this instead</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18j18gb/if_you_experience_lifting_with_soft_gel_tips_even/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>18j0pyk</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Green nails first time</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cfdjh5xxsg6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>18j0g6y</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>I love him I love the glitter on my nails!!</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ckpwyqc9qg6c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>18j0g9x</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Got my nails done in Japan a lifelong dream</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18j0g9x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>18j05kg</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Used some loose sequins</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vziie5nxng6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>18j04co</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Is the aura looking good?</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pnukrzwnng6c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>18il4t7</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>really just need to rant…</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18il4t7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>18ipzxc</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Acrylic Nails Removal Question</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ipzxc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>18issp2</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Update: Holiday Redo!</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18issp2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>18ivpqj</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Your favorite insta account for nail inspo?</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18ivpqj/your_favorite_insta_account_for_nail_inspo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>18izb32</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Winter Nails</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6frklro1gg6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>18iziop</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>my christmas nails i did ft my ex</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r4u5xmg5ig6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>18iz5dt</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>How much would you pay for this set??</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2y3z6klgeg6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>18iwkl9</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Christmas Nails! 🎄❤️💚</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v4scoc8fkf6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>18iw50m</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>I'm pretty new to getting rubber base gel done. I loved them, but really open to hear if this looks good.</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18iw50m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>18iviv5</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>I love cow print!</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zw0e51uf6f6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>18iv86e</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>❄️🎅</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/91l29o5l2f6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>18jj4u0</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Mooncat Christmas Nails ✨🎄</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jj4u0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>18ja4ha</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Christmas time!</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wp3363exvi6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>18ji5rz</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Tis the season mani</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ji5rz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>18jhut6</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>ILNP Overcast Collection Skittles Manicure</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18jhut6/ilnp_overcast_collection_skittles_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>18jhmti</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Comparison Swatch Request - KBShimmer "Wrap It Up" and BKL "Still No F*cking Excuse"</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18jhmti/comparison_swatch_request_kbshimmer_wrap_it_up/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>18jh1p5</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Sweet Pea by ILNP 🎀 The perfect nude pink with a pop of holo ✨</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jh1p5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>18jgam8</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>UK shipping: Rainbow Connection vs buying direct from brands?</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18jgam8/uk_shipping_rainbow_connection_vs_buying_direct/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>18jg6t6</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Holo Taco - Plumb Luck</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7pe0bx8wak6c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>18jfst0</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Mooncat - Sabertooth is the perfect backdrop for a winter wonderland!</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r79qcgi67k6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>18jfr1u</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Nails so bright they disrupt my circadian rhythm 🌙✨</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jfr1u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>18jfq04</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Surviving this Summer heatwave</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jfq04</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>18jf8hh</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Nail P-anukah</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jf8hh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>18jf7de</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Cirque Colors Chiffon</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3e1rde0t1k6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>18jesg0</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>A holo-day mani!</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z6rgrex2yj6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>18jeoji</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>What is going on with me and INLP?</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5qjxzls6xj6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>18jedn2</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Requesting swatches?</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18jedn2/requesting_swatches/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>18je2ba</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Struggling with velvet nails</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wdy1ebwxrj6c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>18jd8r2</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>So…. ILNP is the best brand, right?</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18jd8r2/so_ilnp_is_the_best_brand_right/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>18jcytw</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Chrome powder on lacquer is my white whale. Progress!</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jcytw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>18jcjxe</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Finally got my BKL black friday order so I had to use a few of the polishes for my current mani</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jcjxe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>18jcec5</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Lumen Krampus Sack</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jcec5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>18jc4ex</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Sparkles count as festive nails, right?</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i4ek85blbj6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>18jb8d7</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Cirque Colors Illusion Collection</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5o88rbpn4j6c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>18jb3qe</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Friday Confetti 🎉</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jb3qe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>18jawnc</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cirque - paradox </t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6cs7usl12j6c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>18japps</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Mooncat - Bottled Rage 👿</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18japps</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>18jan5u</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>pearls on mars🦪🪐</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/khxe9mkyzi6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>18j9udo</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>ILNP Bitten</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ans8u4flti6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>18j9i5o</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>I'm oiling, I'm filing, I'm oiling...how do I keep this from happening yet again?</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nu7glr4uqi6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>18j9csv</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Progress after 1 year of growth!</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18j9csv/progress_after_1_year_of_growth/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>18j8e54</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>ISN - I scream holo</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zgw09q5thi6c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>18j87ib</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Obsessed with this polish</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18j87ib</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>18j7bb7</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Decided to swatch my recently-expanded collection</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18j7bb7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>18j6nqg</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Trying out jelly &amp; sandwich 💎 💙</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cw8yv9tb4i6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>18j6ivd</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Mooncat Mermaid Bait</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/my2s6bx93i6c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>18j643l</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>OPI Malaga Wine</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18j643l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>18j5cox</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Matte or glossy?</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18j5cox</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>18j5bjm</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>First time trying Mooncat's House of Hades</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18j5bjm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>18j51k0</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Horizontal Dip in Nail?</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5sv3d9btrh6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>18j4794</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Death metal concert tonight so thought I'd try to fit in</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/te00uky5lh6c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>18j409x</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Tech filed free edge immediately after my shellac mani pedi</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18j409x/tech_filed_free_edge_immediately_after_my_shellac/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>18j3mn7</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>I've been collecting polish for 16 years and this is my new all time favorite</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18j3mn7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>18j3d57</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>I need to report a murder 😭💀</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nqs13taleh6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>18j3a2z</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>First set of Christmas nails are still hanging in there after almost two weeks</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l1gpykixdh6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>18j33qk</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Opi/Painted Polish ...</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18j33qk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>18j32zb</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Beginner Essentials stocking stuffer for my Fiancee</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18j32zb/beginner_essentials_stocking_stuffer_for_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>18j2yf5</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>It’s giving fancy themed Christmas gift wrap vibes</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n1aao6icbh6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>18j2eyt</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Longest they’ve been probably ever - before care and after mooncat polish and oil. Help with dryness!</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18j2eyt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>18j2ajb</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>glittery topper recommendation</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c780kalz5h6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>18j1zq4</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Biab and peel off base</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18j1zq4/biab_and_peel_off_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>18j1u72</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>DVN Dill Weed + Wildflowers + Cornflower Milky Nails</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ea07ol22h6c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>18j1npl</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>{PR} In Love With Red Reflective 😍</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0d2thahw0h6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>18j0z12</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18j0z12</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>18j0wit</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Velvet nails magnets</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18j0wit</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>18j0tby</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Blue Velvet nails featuring freshly oiled cuticles</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i2c6lbgotg6c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>18j0jqk</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cameras can't do this one justice </t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h1tw6dqcrg6c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>18iymvw</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Mooncat - Blame My Star Sign</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18iymvw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>18ix6kb</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>A blue jelly sandwich! Orly bonder, Picture polish North Poke, two coats alternating with INLP My private rainbow, Seche Vite</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2qiouuomrf6c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>18ivvkg</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Is a Nail Polish Tray Worth It?</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18ivvkg/is_a_nail_polish_tray_worth_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>18jjj3f</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Moonlight</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3wmatmfy7l6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>18jjgfn</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>hi everyone .</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rapxqrm77l6c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>18jinle</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Got them when the Barbie movie was out loved what my friend did. What style should I get next I need ideas!!</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hrgw9ss2zk6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>18ji5en</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>So happy with this ombré!</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ji5en</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>18jhjhr</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did mom's Christmas nails! </t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qln7zb90ok6c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>18jeesy</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Week old acrylics i did on myself (beginner]</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f0yqrqltuj6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>18j7nsx</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18j7nsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>18j4r6p</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Christmas Nails Thanks to Hubby</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5869ah1jph6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>18j2966</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Candy cane nails ❤️🍬</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r3suz4zo5h6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>18j07jf</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Nails I did myself</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18j07jf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>18j06p4</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Sequined</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d0cl91z7og6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Dec 17 08:07:25 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_12_17.xlsx
+++ b/data/2023_12_17.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1103"/>
+  <dimension ref="A1:C1264"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19184,6 +19184,2743 @@
         </is>
       </c>
     </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>18kc1vu</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>⛄ Snowflakes ❄️ First time trying a freehand design on gel nails!</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u2rjmgz66t6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>18kbyfy</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Sets over the last three months</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18kbyfy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>18kbgsk</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Christmas nails 🎁</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zpv2ee7vys6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>18kaokq</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Holly Jolly Xmas Mani</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18kaokq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>18ka6qq</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>A set of Christmas nails.</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9huj4hrbks6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>18k9u90</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Classic frenchies have my heart 🤍</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7rwtzrrhgs6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>18k9ss7</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>🫐</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18k9ss7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>18k9q59</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Default Xmas=metallic</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ydnfi17afs6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>18k9fzd</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>(Born male) Any tips on how to prevent dead skin at the base and edges of my nails, shape my nails to be more oval, and strengthen them? Absolutely new to this so any help is appreciated!</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gakpw0cbcs6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>18k9c1s</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m in love with this red 🎄 </t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/coh9f7v5bs6c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>18k9b9z</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Coffin painted white tips 🤍</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18k9b9z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>18k9aca</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Having trouble finding big enough fake nails for my hands. Male 37 years old.</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18k9aca/having_trouble_finding_big_enough_fake_nails_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>18k5um1</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Can't get polish to last more than 24 hours without chipping or coming off at the tips</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18k5um1/cant_get_polish_to_last_more_than_24_hours/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>18k9700</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>First set in 3 months missed this so much 😩</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18k9700</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>18k0vjb</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Why does my gel polish keep chipping no matter what I do?</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18k0vjb/why_does_my_gel_polish_keep_chipping_no_matter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>18jvyll</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>I want to do my own nails, what do I need?</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nwtvjrxeyo6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>18k92qm</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Koi fish nails</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/udxbl1lg8s6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>18k8snw</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Christmas nails 🎄</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/827r6kmi5s6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>18k8gnp</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>If Ballet Core and Miffy had a baby</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/imknb8yy1s6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>18k81t2</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Nail Biting/Picking advice</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18k81t2/nail_bitingpicking_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>18k8145</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Gold baby.</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18k8145</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>18k7750</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Light Pink Cat Eye 💗</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l04rt7wtor6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>18k75kx</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>First Christmas mani of the season! 💖🎄</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7xjlyf8dor6c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>18k6zt5</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>I’m not a nail tech, I’ve just been doing my own nails for fun for 3+ years, this is my progress</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18k6zt5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>18k6zcl</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>square or almond?</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18k6zcl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>18k6vw9</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Trying to be festive without using red or green ✨</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/szqug45qlr6c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>18k6ral</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Slowly getting better at doing my own gel extensions….</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ecwjo1jfkr6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>18k67jb</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>🎄💚🍀🌲</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/silnv2t5fr6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>18k5xuk</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Glitter over the grow out</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18k5xuk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>18k5mgt</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>My artist is amazing. Freehand 💯</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ho0kq0q9r6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>18k5fp5</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>First fill.. are my natural nails lifting from my natural nail bed? (The acrylic is on fine)</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a1a853hy7r6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>18k5bwk</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Have been practicing using builder gel on my natural nails, I’m very proud of this set!</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18k5bwk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>18k59d9</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Really simple but I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0qfewou86r6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>18k51ki</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>My rainbow snowflake nails I did on myself!</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k75wl1p94r6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>18k4rhg</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Holiday Dark Green Sparkle Nails</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18k4rhg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>18k4qok</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Happy Holidays</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f9fvwpgj1r6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>18k4d9y</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Winter themed nails 🤍</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9awf5rh9yq6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>18k42fq</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Does anyone have any shape recommendations for my flat/wide nails?</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k2wblyqlvq6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>18k41wd</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Holiday Nails!</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z6lt8hsevq6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>18k3tsx</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Hello Kitty Pink Winter Set ❄️ 🎀</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18k3tsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>18k3rlf</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>I’m such a snob when it comes to pedicures! Anyone else? I kinda hate it /:</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mxkkq2fysq6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>18k3qkw</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Can my middle finger ever get to oval shape? I bring the edges in and it just turns the nail into a circle:( my beds are so wide:/</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wk8iemipsq6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>18k2z0m</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Clean Girl, but make it Winter ✨❄️</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/exdrkag1mq6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>18k2wdg</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>I’ve been filing chopsticks and using them to push my cuticles back.</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sz7tk25glq6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>18k2umv</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>my favorite so far!</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j76hq7wzkq6c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>18k2tmd</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8th3y3hrkq6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>18k2qy2</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Embracing snowy season ❄️</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4uiv4am4kq6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>18k2gwx</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Did my own nails and loving the white</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sin3g7iphq6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>18k2gqp</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Different not sure how i feel about them.. made up the design as i went, thoughts?</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18k2gqp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>18k21mn</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Dreaming of a White Christmas.....</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18k21mn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>18k1qa7</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Birthday set :)</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j0ggei8ebq6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>18k1ft1</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Strawberries and oranges 🍓🍊</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18k1ft1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>18k1e44</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>i did my own acrylics.. any tips?</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0u78x6kf8q6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>18k1c4p</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Christmas adjacent! (Dark green not black!)</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fhgvpu0y7q6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>18k19fh</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>My first time using polygel. How’d i do?</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18k19fh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>18k11wq</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8mxqnwee5q6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>18k0l7q</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>I think this is my favorite set I’ve done so far! Love these colors.</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18k0l7q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>18jxg9l</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Winter specials ❄️</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jxg9l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>18jz3ww</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>attempted some multi-nail scenery... my eyes are crying 😂 Can anyone guess what film?</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jz3ww</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>18k0fy1</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Magnetic accent nail</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8g98wm590q6c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>18jxxiw</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Nail Education for 15 Year Old</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18jxxiw/nail_education_for_15_year_old/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>18jzzvb</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>To redo, or not to redo? Christmas is comin'.</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jssh1ngdwp6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>18jztwh</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Feeling Festive</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aluwy6uxup6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>18jzs77</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Resting Grinch Face from 12 Days of Double Dipp’d Christmas</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/prcon08jup6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>18jzjy6</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Nail Strengthener: yay or nay?</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dgam0t5lsp6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>18jzixy</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Are my nails stuck forever? (removal)</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18jzixy/are_my_nails_stuck_forever_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>18jyed5</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>New Nail of the Month!</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uycfw29mip6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>18jy8ez</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Christmas nails 🎄❤️</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/56w4czwbhp6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>18jxs7l</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>tiny little claws</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jxs7l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>18jxqzx</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Winter nails!</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v6anbkpcdp6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>18jxpzx</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Ombre French nails ✨️</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jxpzx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>18jx92u</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Nails!</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jx92u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>18jx2a3</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Little bit of soft razzle dazzle✨️</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jx2a3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>18jwpfk</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Just a simple (and short) gold metallic set for the week before Christmas.</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pclk10ta4p6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>18jwa3g</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>“French Tip” cat eye polish. Love it!</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/609kvjgz0p6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>18jw51e</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>My boyfriend came up with a great idea for magnetizing my nails</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cjduyhfuzo6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>18jw4h6</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Maybe a boring post but I thought my tech did such a perfect job with this classic French - SNS on natural nails.</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jw4h6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>18jvw0u</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Cost for refill?</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18jvw0u/cost_for_refill/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>18jvtxp</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Broke two nails, do I trim the rest?</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18jvtxp/broke_two_nails_do_i_trim_the_rest/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>18jvlw8</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Do you tip for getting dip powder removed?</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18jvlw8/do_you_tip_for_getting_dip_powder_removed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>18jurhy</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Bloody Christmas, Krampus, Hail Santa snowflake candy cane nails!</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j09lioxeoo6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>18jty7b</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Found this picture while surfing on Pinterest. What are these? Can they be attached on nails? Where can I get them? :D</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lstukjs6ho6c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>18jv4fi</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Some understated festive nails</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jv4fi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>18jug7z</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Christmas and birthday nails! ✨December babies unite✨</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jug7z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>18ju22w</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>What Am I Doing Wrong...</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18ju22w/what_am_i_doing_wrong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>18jtvw4</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Red chrome for Christmas ❤️</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sfvtgvstgo6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>18jtmsz</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Christmas nails! ✨</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i4xki5ujeo6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>18jtmr1</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Ready for cookie baking!</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yk97kaugeo6c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>18jp4t7</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Question</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18jp4t7/question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>18jp1vd</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Nails stained with foundation</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jp1vd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>18jnavn</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>How do I prevent this gap between the extension and my nail plate? (Using forms with builder gel)</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v0qz740qgm6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>18jl8fp</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>how do you take contacts out with short nails</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18jl8fp/how_do_you_take_contacts_out_with_short_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>18jsy98</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Getting my first time winter themed nails</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jsy98</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>18jsrbb</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>How do they look?</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jsrbb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>18js4sq</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Did gel x for the first time!</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18js4sq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>18jryet</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>@alicasmd</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bfvn41t9zn6c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>18jraku</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Winter Magic ❄️</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jraku</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>18jqrds</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Black Christmas 🖤 🎄</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9bt7i4olnn6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>18jqa5v</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>First time trying french tips</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wo7a77hain6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>18jppsh</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Black holiday nails!</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1uum4mbqbn6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>18kb1o1</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Sassy Sauce - Serpent Queen</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18kb1o1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>18kahmj</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Safe to use cheap gel (Beetles etc) on press-ons?</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18kahmj/safe_to_use_cheap_gel_beetles_etc_on_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>18k3d1h</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Halloween polish + summer polish = sorta Christmas?</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18k3d1h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>18k8px2</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>What are your fav chunky glitters?</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18k8px2/what_are_your_fav_chunky_glitters/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>18k8jso</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>I found a way to take a picture of both hands myself…..😂</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qcru34ux2s6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>18k8j9a</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Yet another Velvet effect</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18k8j9a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>18k8bgl</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Love Spell by Holo Taco</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sxbxkr4c0s6c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>18k892a</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>mooncat flight of the monarchs 🤩🤩</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18k892a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>18k81l2</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Milky Palette Cleanser</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18k81l2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>18k7yvz</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Recent Purchase Skittle Mani</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18k7yvz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>18k7hrf</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Christmas Mix</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rm0xy5bsrr6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>18k736x</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>First Christmas mani of the season! 💖🎄</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tysg157lnr6c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>18k69am</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Christmas Classic</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xd96dpxmfr6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>18k6216</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Is there a nail polish that looks close to this? The same colors and textures?</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/36bhwplpdr6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>18k5sif</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>What shape (rounded, squoval, or coffin ) would be ideal for my nails’s amount of c curve?</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18k5sif</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>18k4se6</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Dark Green Holiday Nails</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18k4se6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>18k4mru</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Help IDing Lumen Mystery Polishes?</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18k4mru</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>18k4ma2</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Who are you?</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18k4ma2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>18k2yfi</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>lazy cloud cover up over my chipping</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18k2yfi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>18k2mhp</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Dusty Rose</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j759xef2jq6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>18k2hpl</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Gift Wrap Nails 🎁</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18k2hpl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>18k22l0</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>KBShimmer Pool Shark</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18k22l0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>18k0tmc</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Moody Blue - with a bit of spritz</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18k0tmc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>18k05no</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Desperately trying to force myself into the Christmas spirit (inc. some grinchy shrinkage 🫠)</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r4gpkkirxp6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>18jzsx6</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Snowflake vibes ❄️</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jzsx6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>18jzivu</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Nail Atrengthener: yay or nay?</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lyxf7r5dsp6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>18jz8c6</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Sheer duochrome!</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jz8c6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>18jz4uo</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>DIY possible?</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hfh4d1r4pp6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>18jz3v4</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Started but unsure where to carry on?</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jz3v4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>18jz0dw</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Recording studio nails</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iprg88wznp6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>18jyf2u</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Any ideas for fun gel nail art? I attached a pic of the accessories I have :)</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jyf2u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>18jy7cw</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Cirque Rothko Red + Emily de Molly Gravity Drive</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kmykzrq2hp6c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>18jy3it</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Lone Pine 🌲✨</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jy3it</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>18jxpvs</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>How do you all make your nails look so NEAT? What am I doing wrong?</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18jxpvs/how_do_you_all_make_your_nails_look_so_neat_what/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>18jxk6o</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Happy Holidays!</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cgp3856qbp6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>18jxfld</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Holiday nails</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jxfld</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>18jwxs1</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Ranking all of the nail polish brands I tried in 2023: The ‘Meh’ Chapter</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jwxs1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>18jwego</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Help me find a cuticle nipper that actually works 😭</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18jwego/help_me_find_a_cuticle_nipper_that_actually_works/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>18jv6bv</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>ILNP - Dear Santa</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/um0gxs6xro6c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>18juz31</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>ILNP - Carbon 🤩</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18juz31</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>18juopt</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Got a compliment for my nail polish at the airport</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18juopt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>18ju5xe</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Warm &amp; Spicy</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wsz35t3eio6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>18jtnl6</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>ILNP Diablo for the Holidays</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/51d8l4nreo6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>18jreoc</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Rarely a polish leaves me speechless 🤯 Spectacular!</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z7u98cu5un6c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>18jpkab</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>set of nails i just painted!!</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jpkab</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>18jo0tl</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>I love this color!!!</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d8kjf1c6qm6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>18jnv7t</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Matchy no matchy palette cleanser before the holidays start</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jnv7t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>18jnnt0</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Strengthener turns nails blueish?</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18jnnt0/strengthener_turns_nails_blueish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>18jn0tm</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>I'm starting over and trying to have all my nails as healthy as possible, looking for advice on the ones that are dry/peeling on the tips-</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18jn0tm/im_starting_over_and_trying_to_have_all_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>18k7vhk</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Just finished this Christmas set. I am in love. 🥰</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p0y2icgnvr6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>18k77dc</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Bouncy little Christmas lights 💖🎄</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wxxrc5rvor6c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>18k2huc</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>I did another thing!!</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lf6gflrxhq6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>18k144q</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>First time using charms!</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zsskfxh06q6c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>18jzw0i</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>This weeks nails I did for my friend</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/264fdslgvp6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>18jywwg</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>I love the nails I did today. WE NEVER SETTLE FOR BRIGHTNESS 💎💎💎</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ku8aj69np6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>18jyiu4</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>new nail by Sophie's Nail Studio</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bspxb0bmjp6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>18jwz0a</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Christmas candy nails 💖💅🏼</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jwz0a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>18jw3jv</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>This week’s Christmas nails, what y’all think?</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6tiiy9rizo6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>18juxss</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>101 Dalmations - Second attempt</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zysr0xrvpo6c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>18jsrie</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Oh Christmas tree!</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zstl1w1r6o6c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>18jqp25</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Any ideas for fun gel nail art? I attached a pic of the accessories I have :)</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18jqp25</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>